<commit_message>
Made figures for all stuff
</commit_message>
<xml_diff>
--- a/results/Results Overview.xlsx
+++ b/results/Results Overview.xlsx
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="89">
   <si>
     <t>Method</t>
   </si>
@@ -356,9 +356,6 @@
     <t xml:space="preserve">time average (minutes) </t>
   </si>
   <si>
-    <t>Time (min)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Error </t>
   </si>
   <si>
@@ -397,6 +394,18 @@
   <si>
     <t>My validation runs</t>
   </si>
+  <si>
+    <t>sni</t>
+  </si>
+  <si>
+    <t>Time Standard Deviation</t>
+  </si>
+  <si>
+    <t>Time Average (min)</t>
+  </si>
+  <si>
+    <t>Error Standard Deviation</t>
+  </si>
 </sst>
 </file>
 
@@ -406,9 +415,9 @@
     <numFmt numFmtId="164" formatCode="0.00&quot;s&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0\ &quot;min&quot;"/>
     <numFmt numFmtId="166" formatCode="0.0\ &quot;h&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.0000%"/>
-    <numFmt numFmtId="172" formatCode="0.000%"/>
-    <numFmt numFmtId="174" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="168" formatCode="0.000%"/>
+    <numFmt numFmtId="169" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1216,6 +1225,26 @@
     <xf numFmtId="165" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1297,26 +1326,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1365,87 +1374,8 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Wu, 2023</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="percentage"/>
-            <c:noEndCap val="0"/>
-            <c:val val="2.98"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Summary!$B$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Summary!$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000%</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3.0200000000000001E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-73B0-43D3-8F98-47CE944C5AA2}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="1"/>
           <c:tx>
             <c:v>Validation</c:v>
           </c:tx>
@@ -1563,6 +1493,85 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Wu, 2023</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:alpha val="96000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="2.98"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Summary!$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Summary!$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000%</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.0200000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-73B0-43D3-8F98-47CE944C5AA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1606,7 +1615,7 @@
                 <a:pPr>
                   <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1636,7 +1645,7 @@
               <a:pPr>
                 <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1"/>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1653,14 +1662,12 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="dk1"/>
             </a:solidFill>
-            <a:round/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="800000"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1673,9 +1680,9 @@
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1731,7 +1738,7 @@
                 <a:pPr>
                   <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1768,7 +1775,7 @@
               <a:pPr>
                 <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1"/>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1785,14 +1792,12 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="dk1"/>
             </a:solidFill>
-            <a:round/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="800000"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1805,9 +1810,9 @@
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -1818,9 +1823,15 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1839,9 +1850,13 @@
       </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -1852,7 +1867,7 @@
           <a:pPr>
             <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
@@ -1889,7 +1904,7 @@
       <a:pPr>
         <a:defRPr sz="1100">
           <a:solidFill>
-            <a:schemeClr val="tx1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -3277,7 +3292,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$C$14</c15:sqref>
@@ -3294,7 +3309,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-218A-4BD3-A029-3BA8A5E835A0}"/>
                   </c:ext>
@@ -3619,10 +3634,10 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Wu, 2023</c:v>
+            <c:v>Validation</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3646,6 +3661,99 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>1.03</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(Summary!$E$6,Summary!$E$14,Summary!$E$13,Summary!$E$20,Summary!$E$7:$E$8)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.0000%">
+                  <c:v>3.1219044989073814E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8129160408279955E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3468408479312121E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20228016901530585</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="0.0000%">
+                  <c:v>8.4485917713194789E-4</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.0000%">
+                  <c:v>1.496013399019277E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-33FF-4BC0-8E33-9BF9D65C9276}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Wu, 2023</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:dPt>
             <c:idx val="0"/>
             <c:marker>
@@ -3653,11 +3761,15 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
                   </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
@@ -3677,11 +3789,15 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
                   </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
@@ -3701,11 +3817,15 @@
               <c:size val="5"/>
               <c:spPr>
                 <a:solidFill>
-                  <a:schemeClr val="accent2"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="accent2"/>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
                   </a:solidFill>
                 </a:ln>
                 <a:effectLst/>
@@ -3758,77 +3878,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-33FF-4BC0-8E33-9BF9D65C9276}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Validation</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="3"/>
-              <c:pt idx="0">
-                <c:v>1.03</c:v>
-              </c:pt>
-              <c:pt idx="1">
-                <c:v>2</c:v>
-              </c:pt>
-              <c:pt idx="2">
-                <c:v>3</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>(Summary!$E$6,Summary!$E$14,Summary!$E$20)</c:f>
-              <c:numCache>
-                <c:formatCode>0.000%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0" formatCode="0.0000%">
-                  <c:v>3.1219044989073814E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.8129160408279955E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.20228016901530585</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-33FF-4BC0-8E33-9BF9D65C9276}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3936,10 +3985,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -3952,7 +3998,7 @@
             <a:pPr>
               <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -4066,14 +4112,12 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
+              <a:schemeClr val="dk1"/>
             </a:solidFill>
-            <a:round/>
+            <a:prstDash val="solid"/>
+            <a:miter lim="800000"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4086,9 +4130,9 @@
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4101,11 +4145,55 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.77529744472124906"/>
+          <c:y val="0.42132871782596509"/>
+          <c:w val="0.18743661573805406"/>
+          <c:h val="0.15412811309448654"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -14869,10 +14957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H22"/>
+  <dimension ref="B1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="J13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14885,22 +14973,25 @@
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="197" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="170" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B2" s="171" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="198" t="s">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C3" s="178" t="s">
+        <v>78</v>
+      </c>
+      <c r="N3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="205" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
         <v>69</v>
       </c>
@@ -14908,7 +14999,7 @@
         <v>71</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>12</v>
@@ -14916,296 +15007,296 @@
       <c r="F4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="209" t="s">
+      <c r="G4" s="182" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="199">
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="172">
         <v>2000</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="200">
+      <c r="E5" s="173">
         <v>3.0200000000000001E-2</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="208" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" s="208" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="199">
+      <c r="G5" s="181" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="181" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" s="172">
         <v>2000</v>
       </c>
-      <c r="C6" s="204">
+      <c r="C6" s="177">
         <v>15.223050000000001</v>
       </c>
       <c r="D6" s="167">
         <v>1.5421363771837118</v>
       </c>
-      <c r="E6" s="201">
+      <c r="E6" s="174">
         <v>3.1219044989073814E-2</v>
       </c>
       <c r="F6" s="167">
         <v>1.9267628015677642E-2</v>
       </c>
-      <c r="G6" s="207">
+      <c r="G6" s="180">
         <f>(E6-E5)/(AVERAGE(E5:E6))</f>
         <v>3.3183355073498663E-2</v>
       </c>
-      <c r="H6" s="207">
+      <c r="H6" s="180">
         <f>(E6-E5)/E5</f>
         <v>3.3743211558735518E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="199">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="172">
         <v>5000</v>
       </c>
-      <c r="C7" s="204">
+      <c r="C7" s="177">
         <v>37.659633333333332</v>
       </c>
       <c r="D7" s="167">
         <v>4.5057002438886391</v>
       </c>
-      <c r="E7" s="201">
+      <c r="E7" s="174">
         <v>8.4485917713194789E-4</v>
       </c>
       <c r="F7" s="167">
         <v>4.6608038923739314E-4</v>
       </c>
-      <c r="G7" s="208" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="208" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="199">
+      <c r="G7" s="181" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="181" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="172">
         <v>10000</v>
       </c>
-      <c r="C8" s="204">
+      <c r="C8" s="177">
         <v>63.890166666666666</v>
       </c>
       <c r="D8" s="167">
         <v>7.0136932631024571</v>
       </c>
-      <c r="E8" s="201">
+      <c r="E8" s="174">
         <v>1.496013399019277E-4</v>
       </c>
       <c r="F8" s="167">
         <v>7.0086486756693633E-5</v>
       </c>
-      <c r="G8" s="208" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="208" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="205" t="s">
+      <c r="G8" s="181" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="181" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C10" s="178" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="F11" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G11" s="206" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="179" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="199" t="s">
-        <v>76</v>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" s="172" t="s">
+        <v>75</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
-      <c r="E12" s="202">
+      <c r="E12" s="175">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F12" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="208" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="208" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="199" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="204">
+        <v>76</v>
+      </c>
+      <c r="G12" s="181" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="181" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="172" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="177">
         <v>27.373756788794147</v>
       </c>
       <c r="D13" s="167">
         <v>1.0091068244167525</v>
       </c>
-      <c r="E13" s="203">
+      <c r="E13" s="176">
         <v>9.3468408479312121E-2</v>
       </c>
       <c r="F13" s="167">
         <v>0.22164482527331889</v>
       </c>
-      <c r="G13" s="207">
+      <c r="G13" s="180">
         <f>(E13-E12)/(AVERAGE(E12:E13))</f>
         <v>1.9914592335560317</v>
       </c>
-      <c r="H13" s="207">
+      <c r="H13" s="180">
         <f>(E13-E12)/E12</f>
         <v>466.34204239656054</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="199" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="204">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="172" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="177">
         <v>709.57799999999997</v>
       </c>
       <c r="D14" s="167">
         <v>387.22900119944109</v>
       </c>
-      <c r="E14" s="203">
+      <c r="E14" s="176">
         <v>7.8129160408279955E-4</v>
       </c>
       <c r="F14" s="167">
         <v>6.8766974675303508E-4</v>
       </c>
-      <c r="G14" s="207">
+      <c r="G14" s="180">
         <f>(E14-E12)/(AVERAGE(E12,E14))</f>
         <v>1.1847479417214115</v>
       </c>
-      <c r="H14" s="207">
+      <c r="H14" s="180">
         <f>(E14-E12)/E12</f>
         <v>2.9064580204139978</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="205" t="s">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C16" s="178" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
       <c r="C17" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="F17" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="206" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="179" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="199" t="s">
-        <v>76</v>
+      <c r="B18" s="172" t="s">
+        <v>75</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="202">
+      <c r="E18" s="175">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="208" t="s">
-        <v>80</v>
-      </c>
-      <c r="H18" s="208" t="s">
-        <v>80</v>
+        <v>77</v>
+      </c>
+      <c r="G18" s="181" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="181" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="199" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="204">
+      <c r="B19" s="172" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="177">
         <v>72.482200707579878</v>
       </c>
       <c r="D19" s="167">
         <v>62.426871740883726</v>
       </c>
-      <c r="E19" s="203">
+      <c r="E19" s="176">
         <v>0.17557805468751683</v>
       </c>
       <c r="F19" s="167">
         <v>7.0928462417294655E-2</v>
       </c>
-      <c r="G19" s="207">
+      <c r="G19" s="180">
         <f>(E19-E18)/(AVERAGE(E18:E19))</f>
         <v>1.9931770907852489</v>
       </c>
-      <c r="H19" s="207">
+      <c r="H19" s="180">
         <f>(E19-E18)/E18</f>
         <v>584.2601822917228</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="199" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="204">
+      <c r="B20" s="172" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="177">
         <v>445.01751002695778</v>
       </c>
       <c r="D20" s="167">
         <v>213.20960078680412</v>
       </c>
-      <c r="E20" s="203">
+      <c r="E20" s="176">
         <v>0.20228016901530585</v>
       </c>
       <c r="F20" s="167">
         <v>0.10054384794661249</v>
       </c>
-      <c r="G20" s="207">
+      <c r="G20" s="180">
         <f>(E20-E18)/(AVERAGE(E18,E20))</f>
         <v>1.9940764191982221</v>
       </c>
-      <c r="H20" s="207">
+      <c r="H20" s="180">
         <f>(E20-E18)/E18</f>
         <v>673.26723005101962</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="210" t="s">
-        <v>83</v>
+      <c r="B22" s="183" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -15238,37 +15329,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="185" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="129"/>
       <c r="C1" s="129"/>
-      <c r="D1" s="168" t="s">
+      <c r="D1" s="184" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="168"/>
-      <c r="F1" s="168"/>
-      <c r="G1" s="168"/>
-      <c r="H1" s="168"/>
-      <c r="I1" s="168"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+      <c r="G1" s="184"/>
+      <c r="H1" s="184"/>
+      <c r="I1" s="184"/>
       <c r="J1" s="130"/>
-      <c r="K1" s="173" t="s">
+      <c r="K1" s="189" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="171"/>
-      <c r="R1" s="174" t="s">
+      <c r="L1" s="189"/>
+      <c r="M1" s="189"/>
+      <c r="N1" s="189"/>
+      <c r="O1" s="189"/>
+      <c r="P1" s="189"/>
+      <c r="Q1" s="187"/>
+      <c r="R1" s="190" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="174"/>
-      <c r="T1" s="174"/>
+      <c r="S1" s="190"/>
+      <c r="T1" s="190"/>
     </row>
     <row r="2" spans="1:20" s="7" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="170"/>
+      <c r="A2" s="186"/>
       <c r="B2" s="138" t="s">
         <v>51</v>
       </c>
@@ -15312,7 +15403,7 @@
       <c r="P2" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="172"/>
+      <c r="Q2" s="188"/>
       <c r="R2" s="136" t="s">
         <v>43</v>
       </c>
@@ -15808,7 +15899,7 @@
         <f t="shared" si="0"/>
         <v>39.766666666666666</v>
       </c>
-      <c r="N13" s="195">
+      <c r="N13" s="168">
         <f>M13/60</f>
         <v>0.6627777777777778</v>
       </c>
@@ -16696,7 +16787,7 @@
         <f t="shared" ref="M33:M34" si="2">L33/60</f>
         <v>30.66095550855</v>
       </c>
-      <c r="N33" s="196">
+      <c r="N33" s="169">
         <f>M33/60</f>
         <v>0.51101592514250005</v>
       </c>
@@ -16740,7 +16831,7 @@
         <f t="shared" si="2"/>
         <v>58.543333333333329</v>
       </c>
-      <c r="N34" s="196">
+      <c r="N34" s="169">
         <f>M34/60</f>
         <v>0.97572222222222216</v>
       </c>
@@ -16782,7 +16873,7 @@
         <f>L35/60</f>
         <v>98.1755</v>
       </c>
-      <c r="N35" s="196">
+      <c r="N35" s="169">
         <f t="shared" ref="N35" si="3">M35/60</f>
         <v>1.6362583333333334</v>
       </c>
@@ -18798,40 +18889,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="180" t="s">
+      <c r="A1" s="196" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="177" t="s">
+      <c r="B1" s="193" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="119"/>
-      <c r="D1" s="182" t="s">
+      <c r="D1" s="198" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
-      <c r="H1" s="182"/>
-      <c r="I1" s="182"/>
+      <c r="E1" s="198"/>
+      <c r="F1" s="198"/>
+      <c r="G1" s="198"/>
+      <c r="H1" s="198"/>
+      <c r="I1" s="198"/>
       <c r="J1" s="120"/>
-      <c r="K1" s="183" t="s">
+      <c r="K1" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="183"/>
-      <c r="M1" s="183"/>
-      <c r="N1" s="183"/>
-      <c r="O1" s="183"/>
-      <c r="P1" s="183"/>
-      <c r="Q1" s="184"/>
-      <c r="R1" s="179" t="s">
+      <c r="L1" s="199"/>
+      <c r="M1" s="199"/>
+      <c r="N1" s="199"/>
+      <c r="O1" s="199"/>
+      <c r="P1" s="199"/>
+      <c r="Q1" s="200"/>
+      <c r="R1" s="195" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
+      <c r="S1" s="195"/>
+      <c r="T1" s="195"/>
     </row>
     <row r="2" spans="1:20" s="7" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="181"/>
-      <c r="B2" s="178"/>
+      <c r="A2" s="197"/>
+      <c r="B2" s="194"/>
       <c r="C2" s="121" t="s">
         <v>19</v>
       </c>
@@ -18872,7 +18963,7 @@
       <c r="P2" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="185"/>
+      <c r="Q2" s="201"/>
       <c r="R2" s="145" t="s">
         <v>43</v>
       </c>
@@ -18890,7 +18981,7 @@
       <c r="B3" s="144" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="175" t="s">
+      <c r="C3" s="191" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="31" t="s">
@@ -18940,7 +19031,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="144"/>
-      <c r="C4" s="176"/>
+      <c r="C4" s="192"/>
       <c r="D4" s="37" t="s">
         <v>7</v>
       </c>
@@ -18988,7 +19079,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="144"/>
-      <c r="C5" s="176"/>
+      <c r="C5" s="192"/>
       <c r="D5" s="37" t="s">
         <v>7</v>
       </c>
@@ -19036,7 +19127,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="144"/>
-      <c r="C6" s="176"/>
+      <c r="C6" s="192"/>
       <c r="D6" s="37" t="s">
         <v>7</v>
       </c>
@@ -19084,7 +19175,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="144"/>
-      <c r="C7" s="176"/>
+      <c r="C7" s="192"/>
       <c r="D7" s="37" t="s">
         <v>7</v>
       </c>
@@ -19132,7 +19223,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="144"/>
-      <c r="C8" s="176"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="37" t="s">
         <v>7</v>
       </c>
@@ -19180,7 +19271,7 @@
         <v>18</v>
       </c>
       <c r="B9" s="144"/>
-      <c r="C9" s="176"/>
+      <c r="C9" s="192"/>
       <c r="D9" s="37" t="s">
         <v>7</v>
       </c>
@@ -19228,7 +19319,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="144"/>
-      <c r="C10" s="176"/>
+      <c r="C10" s="192"/>
       <c r="D10" s="37" t="s">
         <v>7</v>
       </c>
@@ -19276,7 +19367,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="144"/>
-      <c r="C11" s="176"/>
+      <c r="C11" s="192"/>
       <c r="D11" s="37" t="s">
         <v>7</v>
       </c>
@@ -19326,7 +19417,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="144"/>
-      <c r="C12" s="176"/>
+      <c r="C12" s="192"/>
       <c r="D12" s="37" t="s">
         <v>7</v>
       </c>
@@ -21003,7 +21094,7 @@
   <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33:Q33"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21021,40 +21112,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="202" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="193" t="s">
+      <c r="B1" s="209" t="s">
         <v>47</v>
       </c>
       <c r="C1" s="93"/>
-      <c r="D1" s="188" t="s">
+      <c r="D1" s="204" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="188"/>
-      <c r="F1" s="188"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
+      <c r="E1" s="204"/>
+      <c r="F1" s="204"/>
+      <c r="G1" s="204"/>
+      <c r="H1" s="204"/>
+      <c r="I1" s="204"/>
       <c r="J1" s="94"/>
-      <c r="K1" s="189" t="s">
+      <c r="K1" s="205" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="189"/>
-      <c r="M1" s="189"/>
-      <c r="N1" s="189"/>
-      <c r="O1" s="189"/>
-      <c r="P1" s="189"/>
-      <c r="Q1" s="190"/>
-      <c r="R1" s="179" t="s">
+      <c r="L1" s="205"/>
+      <c r="M1" s="205"/>
+      <c r="N1" s="205"/>
+      <c r="O1" s="205"/>
+      <c r="P1" s="205"/>
+      <c r="Q1" s="206"/>
+      <c r="R1" s="195" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="179"/>
-      <c r="T1" s="179"/>
+      <c r="S1" s="195"/>
+      <c r="T1" s="195"/>
     </row>
     <row r="2" spans="1:20" s="7" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="187"/>
-      <c r="B2" s="194"/>
+      <c r="A2" s="203"/>
+      <c r="B2" s="210"/>
       <c r="C2" s="95"/>
       <c r="D2" s="96" t="s">
         <v>4</v>
@@ -21093,7 +21184,7 @@
       <c r="P2" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="191"/>
+      <c r="Q2" s="207"/>
       <c r="R2" s="90" t="s">
         <v>43</v>
       </c>
@@ -22519,16 +22610,16 @@
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
       <c r="T30" s="13"/>
-      <c r="AC30" s="192"/>
-      <c r="AD30" s="192"/>
-      <c r="AE30" s="192"/>
-      <c r="AF30" s="192"/>
-      <c r="AG30" s="192"/>
-      <c r="AH30" s="192"/>
-      <c r="AI30" s="192"/>
-      <c r="AJ30" s="192"/>
-      <c r="AK30" s="192"/>
-      <c r="AL30" s="192"/>
+      <c r="AC30" s="208"/>
+      <c r="AD30" s="208"/>
+      <c r="AE30" s="208"/>
+      <c r="AF30" s="208"/>
+      <c r="AG30" s="208"/>
+      <c r="AH30" s="208"/>
+      <c r="AI30" s="208"/>
+      <c r="AJ30" s="208"/>
+      <c r="AK30" s="208"/>
+      <c r="AL30" s="208"/>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -22563,16 +22654,16 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
-      <c r="AC31" s="192"/>
-      <c r="AD31" s="192"/>
-      <c r="AE31" s="192"/>
-      <c r="AF31" s="192"/>
-      <c r="AG31" s="192"/>
-      <c r="AH31" s="192"/>
-      <c r="AI31" s="192"/>
-      <c r="AJ31" s="192"/>
-      <c r="AK31" s="192"/>
-      <c r="AL31" s="192"/>
+      <c r="AC31" s="208"/>
+      <c r="AD31" s="208"/>
+      <c r="AE31" s="208"/>
+      <c r="AF31" s="208"/>
+      <c r="AG31" s="208"/>
+      <c r="AH31" s="208"/>
+      <c r="AI31" s="208"/>
+      <c r="AJ31" s="208"/>
+      <c r="AK31" s="208"/>
+      <c r="AL31" s="208"/>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
@@ -22607,16 +22698,16 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-      <c r="AC32" s="192"/>
-      <c r="AD32" s="192"/>
-      <c r="AE32" s="192"/>
-      <c r="AF32" s="192"/>
-      <c r="AG32" s="192"/>
-      <c r="AH32" s="192"/>
-      <c r="AI32" s="192"/>
-      <c r="AJ32" s="192"/>
-      <c r="AK32" s="192"/>
-      <c r="AL32" s="192"/>
+      <c r="AC32" s="208"/>
+      <c r="AD32" s="208"/>
+      <c r="AE32" s="208"/>
+      <c r="AF32" s="208"/>
+      <c r="AG32" s="208"/>
+      <c r="AH32" s="208"/>
+      <c r="AI32" s="208"/>
+      <c r="AJ32" s="208"/>
+      <c r="AK32" s="208"/>
+      <c r="AL32" s="208"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
@@ -22651,16 +22742,16 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
-      <c r="AC33" s="192"/>
-      <c r="AD33" s="192"/>
-      <c r="AE33" s="192"/>
-      <c r="AF33" s="192"/>
-      <c r="AG33" s="192"/>
-      <c r="AH33" s="192"/>
-      <c r="AI33" s="192"/>
-      <c r="AJ33" s="192"/>
-      <c r="AK33" s="192"/>
-      <c r="AL33" s="192"/>
+      <c r="AC33" s="208"/>
+      <c r="AD33" s="208"/>
+      <c r="AE33" s="208"/>
+      <c r="AF33" s="208"/>
+      <c r="AG33" s="208"/>
+      <c r="AH33" s="208"/>
+      <c r="AI33" s="208"/>
+      <c r="AJ33" s="208"/>
+      <c r="AK33" s="208"/>
+      <c r="AL33" s="208"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>